<commit_message>
Upto All change Code review.
</commit_message>
<xml_diff>
--- a/restapp/Habile_Investak_API_Dictionary_1.1_20170119.xlsx
+++ b/restapp/Habile_Investak_API_Dictionary_1.1_20170119.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="900" windowWidth="20730" windowHeight="11760" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="900" windowWidth="20730" windowHeight="11760" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="8" r:id="rId1"/>
@@ -23,7 +23,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">SUCCESS!$A$1:$K$254</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -7645,12 +7644,7 @@
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:L102" totalsRowShown="0" headerRowDxfId="62" dataDxfId="60" headerRowBorderDxfId="61" tableBorderDxfId="59" totalsRowBorderDxfId="58">
   <autoFilter ref="A1:L102">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="AccountInfo"/>
-        <filter val="OpenOrders"/>
-      </filters>
-    </filterColumn>
+    <filterColumn colId="1"/>
   </autoFilter>
   <tableColumns count="12">
     <tableColumn id="1" name="#" dataDxfId="57"/>
@@ -8023,7 +8017,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -9467,11 +9461,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="H5" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="5" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L8" sqref="L8"/>
+      <selection pane="bottomRight" activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9559,10 +9553,10 @@
         <v>1290</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>4</v>
+        <v>1239</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>4</v>
+        <v>1239</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>150</v>
@@ -9600,10 +9594,10 @@
         <v>1291</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>4</v>
+        <v>1239</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>4</v>
+        <v>1239</v>
       </c>
       <c r="K3" s="6" t="s">
         <v>157</v>
@@ -9641,7 +9635,7 @@
         <v>1292</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>4</v>
+        <v>1239</v>
       </c>
       <c r="J4" s="5" t="s">
         <v>150</v>
@@ -9680,10 +9674,10 @@
         <v>1293</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>4</v>
+        <v>1239</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>4</v>
+        <v>1239</v>
       </c>
       <c r="K5" s="5" t="s">
         <v>150</v>
@@ -9717,10 +9711,10 @@
         <v>1294</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>4</v>
+        <v>1239</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>4</v>
+        <v>1239</v>
       </c>
       <c r="K6" s="6" t="s">
         <v>179</v>
@@ -9756,10 +9750,10 @@
         <v>1295</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>4</v>
+        <v>1239</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>4</v>
+        <v>1239</v>
       </c>
       <c r="K7" s="6" t="s">
         <v>179</v>
@@ -9795,10 +9789,10 @@
         <v>1296</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>4</v>
+        <v>1239</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>4</v>
+        <v>1239</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="6" t="s">
@@ -9834,10 +9828,10 @@
         <v>1314</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>4</v>
+        <v>1239</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>4</v>
+        <v>1239</v>
       </c>
       <c r="K9" s="6" t="s">
         <v>233</v>
@@ -9871,10 +9865,10 @@
         <v>1297</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>4</v>
+        <v>1239</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>4</v>
+        <v>1239</v>
       </c>
       <c r="K10" s="6" t="s">
         <v>233</v>
@@ -9910,10 +9904,10 @@
         <v>1298</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>4</v>
+        <v>1239</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>4</v>
+        <v>1239</v>
       </c>
       <c r="K11" s="6" t="s">
         <v>233</v>
@@ -9947,10 +9941,10 @@
         <v>1299</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>4</v>
+        <v>1239</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>4</v>
+        <v>1239</v>
       </c>
       <c r="K12" s="6" t="s">
         <v>233</v>
@@ -9980,7 +9974,7 @@
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
       <c r="I13" s="6" t="s">
-        <v>4</v>
+        <v>1239</v>
       </c>
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
@@ -10013,10 +10007,10 @@
         <v>1306</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>4</v>
+        <v>1239</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>4</v>
+        <v>1239</v>
       </c>
       <c r="K14" s="6" t="s">
         <v>233</v>
@@ -10050,10 +10044,10 @@
         <v>1307</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>4</v>
+        <v>1239</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>4</v>
+        <v>1239</v>
       </c>
       <c r="K15" s="6" t="s">
         <v>233</v>
@@ -10087,10 +10081,10 @@
         <v>1300</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>4</v>
+        <v>1239</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>4</v>
+        <v>1239</v>
       </c>
       <c r="K16" s="6" t="s">
         <v>233</v>
@@ -10124,10 +10118,10 @@
         <v>1310</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>4</v>
+        <v>1239</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>4</v>
+        <v>1239</v>
       </c>
       <c r="K17" s="6" t="s">
         <v>233</v>
@@ -10161,10 +10155,10 @@
         <v>1308</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>4</v>
+        <v>1239</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>4</v>
+        <v>1239</v>
       </c>
       <c r="K18" s="6" t="s">
         <v>233</v>
@@ -10198,10 +10192,10 @@
         <v>1309</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>4</v>
+        <v>1239</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>4</v>
+        <v>1239</v>
       </c>
       <c r="K19" s="6" t="s">
         <v>233</v>
@@ -10235,10 +10229,10 @@
         <v>1301</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>4</v>
+        <v>1239</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>4</v>
+        <v>1239</v>
       </c>
       <c r="K20" s="6" t="s">
         <v>233</v>
@@ -10272,10 +10266,10 @@
         <v>1312</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>4</v>
+        <v>1239</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>4</v>
+        <v>1239</v>
       </c>
       <c r="K21" s="6" t="s">
         <v>233</v>
@@ -10309,10 +10303,10 @@
         <v>1311</v>
       </c>
       <c r="I22" s="6" t="s">
-        <v>4</v>
+        <v>1239</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>4</v>
+        <v>1239</v>
       </c>
       <c r="K22" s="6" t="s">
         <v>233</v>
@@ -10346,10 +10340,10 @@
         <v>1302</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>4</v>
+        <v>1239</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>4</v>
+        <v>1239</v>
       </c>
       <c r="K23" s="6" t="s">
         <v>233</v>
@@ -10383,10 +10377,10 @@
         <v>1313</v>
       </c>
       <c r="I24" s="6" t="s">
-        <v>4</v>
+        <v>1239</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>4</v>
+        <v>1239</v>
       </c>
       <c r="K24" s="6" t="s">
         <v>233</v>
@@ -10420,10 +10414,10 @@
         <v>1303</v>
       </c>
       <c r="I25" s="6" t="s">
-        <v>4</v>
+        <v>1239</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>4</v>
+        <v>1239</v>
       </c>
       <c r="K25" s="6" t="s">
         <v>233</v>
@@ -10457,10 +10451,10 @@
         <v>1304</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>4</v>
+        <v>1239</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>4</v>
+        <v>1239</v>
       </c>
       <c r="K26" s="6" t="s">
         <v>233</v>
@@ -10494,10 +10488,10 @@
         <v>1305</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>4</v>
+        <v>1239</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>4</v>
+        <v>1239</v>
       </c>
       <c r="K27" s="6" t="s">
         <v>233</v>
@@ -12778,7 +12772,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D99" sqref="D99"/>
+      <selection pane="bottomRight" activeCell="B97" sqref="B97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12835,7 +12829,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="2" spans="1:12" hidden="1">
+    <row r="2" spans="1:12">
       <c r="A2" s="19">
         <v>1</v>
       </c>
@@ -12863,7 +12857,7 @@
       <c r="K2" s="54"/>
       <c r="L2" s="53"/>
     </row>
-    <row r="3" spans="1:12" ht="24" hidden="1">
+    <row r="3" spans="1:12" ht="24">
       <c r="A3" s="19">
         <v>2</v>
       </c>
@@ -12889,7 +12883,7 @@
       <c r="K3" s="15"/>
       <c r="L3" s="46"/>
     </row>
-    <row r="4" spans="1:12" ht="24" hidden="1">
+    <row r="4" spans="1:12" ht="24">
       <c r="A4" s="19">
         <v>3</v>
       </c>
@@ -12915,7 +12909,7 @@
       <c r="K4" s="15"/>
       <c r="L4" s="6"/>
     </row>
-    <row r="5" spans="1:12" hidden="1">
+    <row r="5" spans="1:12">
       <c r="A5" s="19">
         <v>4</v>
       </c>
@@ -12943,7 +12937,7 @@
       <c r="K5" s="15"/>
       <c r="L5" s="6"/>
     </row>
-    <row r="6" spans="1:12" hidden="1">
+    <row r="6" spans="1:12">
       <c r="A6" s="19">
         <v>5</v>
       </c>
@@ -12969,7 +12963,7 @@
       <c r="K6" s="15"/>
       <c r="L6" s="6"/>
     </row>
-    <row r="7" spans="1:12" hidden="1">
+    <row r="7" spans="1:12">
       <c r="A7" s="19">
         <v>6</v>
       </c>
@@ -12997,7 +12991,7 @@
       <c r="K7" s="15"/>
       <c r="L7" s="6"/>
     </row>
-    <row r="8" spans="1:12" hidden="1">
+    <row r="8" spans="1:12">
       <c r="A8" s="19">
         <v>7</v>
       </c>
@@ -13025,7 +13019,7 @@
       <c r="K8" s="15"/>
       <c r="L8" s="6"/>
     </row>
-    <row r="9" spans="1:12" hidden="1">
+    <row r="9" spans="1:12">
       <c r="A9" s="19">
         <v>8</v>
       </c>
@@ -13053,7 +13047,7 @@
       <c r="K9" s="15"/>
       <c r="L9" s="6"/>
     </row>
-    <row r="10" spans="1:12" hidden="1">
+    <row r="10" spans="1:12">
       <c r="A10" s="19">
         <v>9</v>
       </c>
@@ -13083,7 +13077,7 @@
       <c r="K10" s="15"/>
       <c r="L10" s="6"/>
     </row>
-    <row r="11" spans="1:12" hidden="1">
+    <row r="11" spans="1:12">
       <c r="A11" s="19">
         <v>10</v>
       </c>
@@ -13111,7 +13105,7 @@
       <c r="K11" s="15"/>
       <c r="L11" s="6"/>
     </row>
-    <row r="12" spans="1:12" hidden="1">
+    <row r="12" spans="1:12">
       <c r="A12" s="19">
         <v>11</v>
       </c>
@@ -13139,7 +13133,7 @@
       <c r="K12" s="15"/>
       <c r="L12" s="6"/>
     </row>
-    <row r="13" spans="1:12" hidden="1">
+    <row r="13" spans="1:12">
       <c r="A13" s="19">
         <v>12</v>
       </c>
@@ -13169,7 +13163,7 @@
       <c r="K13" s="15"/>
       <c r="L13" s="6"/>
     </row>
-    <row r="14" spans="1:12" hidden="1">
+    <row r="14" spans="1:12">
       <c r="A14" s="19">
         <v>13</v>
       </c>
@@ -13197,7 +13191,7 @@
       <c r="K14" s="15"/>
       <c r="L14" s="6"/>
     </row>
-    <row r="15" spans="1:12" hidden="1">
+    <row r="15" spans="1:12">
       <c r="A15" s="19">
         <v>14</v>
       </c>
@@ -13223,7 +13217,7 @@
       <c r="K15" s="15"/>
       <c r="L15" s="6"/>
     </row>
-    <row r="16" spans="1:12" hidden="1">
+    <row r="16" spans="1:12">
       <c r="A16" s="19">
         <v>15</v>
       </c>
@@ -13249,7 +13243,7 @@
       <c r="K16" s="15"/>
       <c r="L16" s="6"/>
     </row>
-    <row r="17" spans="1:12" ht="24" hidden="1">
+    <row r="17" spans="1:12" ht="24">
       <c r="A17" s="19">
         <v>16</v>
       </c>
@@ -13275,7 +13269,7 @@
       <c r="K17" s="15"/>
       <c r="L17" s="6"/>
     </row>
-    <row r="18" spans="1:12" hidden="1">
+    <row r="18" spans="1:12">
       <c r="A18" s="19">
         <v>17</v>
       </c>
@@ -13303,7 +13297,7 @@
       <c r="K18" s="15"/>
       <c r="L18" s="6"/>
     </row>
-    <row r="19" spans="1:12" hidden="1">
+    <row r="19" spans="1:12">
       <c r="A19" s="19">
         <v>18</v>
       </c>
@@ -13331,7 +13325,7 @@
       <c r="K19" s="15"/>
       <c r="L19" s="6"/>
     </row>
-    <row r="20" spans="1:12" ht="24" hidden="1">
+    <row r="20" spans="1:12" ht="24">
       <c r="A20" s="19">
         <v>19</v>
       </c>
@@ -13359,7 +13353,7 @@
       <c r="K20" s="15"/>
       <c r="L20" s="6"/>
     </row>
-    <row r="21" spans="1:12" ht="24" hidden="1">
+    <row r="21" spans="1:12" ht="24">
       <c r="A21" s="19">
         <v>20</v>
       </c>
@@ -13387,7 +13381,7 @@
       <c r="K21" s="15"/>
       <c r="L21" s="6"/>
     </row>
-    <row r="22" spans="1:12" ht="24" hidden="1">
+    <row r="22" spans="1:12" ht="24">
       <c r="A22" s="19">
         <v>21</v>
       </c>
@@ -13415,7 +13409,7 @@
       <c r="K22" s="15"/>
       <c r="L22" s="6"/>
     </row>
-    <row r="23" spans="1:12" ht="24" hidden="1">
+    <row r="23" spans="1:12" ht="24">
       <c r="A23" s="19">
         <v>22</v>
       </c>
@@ -13443,7 +13437,7 @@
       <c r="K23" s="15"/>
       <c r="L23" s="6"/>
     </row>
-    <row r="24" spans="1:12" hidden="1">
+    <row r="24" spans="1:12">
       <c r="A24" s="19">
         <v>23</v>
       </c>
@@ -13471,7 +13465,7 @@
       <c r="K24" s="15"/>
       <c r="L24" s="6"/>
     </row>
-    <row r="25" spans="1:12" hidden="1">
+    <row r="25" spans="1:12">
       <c r="A25" s="19">
         <v>24</v>
       </c>
@@ -13499,7 +13493,7 @@
       <c r="K25" s="15"/>
       <c r="L25" s="6"/>
     </row>
-    <row r="26" spans="1:12" hidden="1">
+    <row r="26" spans="1:12">
       <c r="A26" s="19">
         <v>25</v>
       </c>
@@ -13527,7 +13521,7 @@
       <c r="K26" s="15"/>
       <c r="L26" s="6"/>
     </row>
-    <row r="27" spans="1:12" hidden="1">
+    <row r="27" spans="1:12">
       <c r="A27" s="19">
         <v>26</v>
       </c>
@@ -13555,7 +13549,7 @@
       <c r="K27" s="15"/>
       <c r="L27" s="6"/>
     </row>
-    <row r="28" spans="1:12" ht="24" hidden="1">
+    <row r="28" spans="1:12" ht="24">
       <c r="A28" s="19">
         <v>27</v>
       </c>
@@ -13583,7 +13577,7 @@
       <c r="K28" s="15"/>
       <c r="L28" s="6"/>
     </row>
-    <row r="29" spans="1:12" ht="24" hidden="1">
+    <row r="29" spans="1:12" ht="24">
       <c r="A29" s="19">
         <v>28</v>
       </c>
@@ -13611,7 +13605,7 @@
       <c r="K29" s="15"/>
       <c r="L29" s="6"/>
     </row>
-    <row r="30" spans="1:12" ht="24" hidden="1">
+    <row r="30" spans="1:12" ht="24">
       <c r="A30" s="19">
         <v>29</v>
       </c>
@@ -13643,7 +13637,7 @@
         <v>1248</v>
       </c>
     </row>
-    <row r="31" spans="1:12" hidden="1">
+    <row r="31" spans="1:12">
       <c r="A31" s="19">
         <v>30</v>
       </c>
@@ -13675,7 +13669,7 @@
         <v>1249</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="24" hidden="1">
+    <row r="32" spans="1:12" ht="24">
       <c r="A32" s="19">
         <v>31</v>
       </c>
@@ -13707,7 +13701,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="36" hidden="1">
+    <row r="33" spans="1:12" ht="36">
       <c r="A33" s="19">
         <v>32</v>
       </c>
@@ -13739,7 +13733,7 @@
         <v>1255</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="48" hidden="1">
+    <row r="34" spans="1:12" ht="48">
       <c r="A34" s="19">
         <v>33</v>
       </c>
@@ -13771,7 +13765,7 @@
         <v>1251</v>
       </c>
     </row>
-    <row r="35" spans="1:12" hidden="1">
+    <row r="35" spans="1:12">
       <c r="A35" s="19">
         <v>34</v>
       </c>
@@ -13805,7 +13799,7 @@
         <v>1256</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="24" hidden="1">
+    <row r="36" spans="1:12" ht="24">
       <c r="A36" s="19">
         <v>35</v>
       </c>
@@ -13837,7 +13831,7 @@
         <v>1252</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="24" hidden="1">
+    <row r="37" spans="1:12" ht="24">
       <c r="A37" s="19">
         <v>36</v>
       </c>
@@ -13869,7 +13863,7 @@
         <v>1248</v>
       </c>
     </row>
-    <row r="38" spans="1:12" hidden="1">
+    <row r="38" spans="1:12">
       <c r="A38" s="19">
         <v>37</v>
       </c>
@@ -13901,7 +13895,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:12" hidden="1">
+    <row r="39" spans="1:12">
       <c r="A39" s="19">
         <v>38</v>
       </c>
@@ -13931,7 +13925,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:12" hidden="1">
+    <row r="40" spans="1:12">
       <c r="A40" s="19">
         <v>39</v>
       </c>
@@ -13961,7 +13955,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="24" hidden="1">
+    <row r="41" spans="1:12" ht="24">
       <c r="A41" s="19">
         <v>40</v>
       </c>
@@ -13991,7 +13985,7 @@
         <v>1253</v>
       </c>
     </row>
-    <row r="42" spans="1:12" hidden="1">
+    <row r="42" spans="1:12">
       <c r="A42" s="19">
         <v>41</v>
       </c>
@@ -14021,7 +14015,7 @@
         <v>1254</v>
       </c>
     </row>
-    <row r="43" spans="1:12" hidden="1">
+    <row r="43" spans="1:12">
       <c r="A43" s="19">
         <v>42</v>
       </c>
@@ -14051,7 +14045,7 @@
         <v>1254</v>
       </c>
     </row>
-    <row r="44" spans="1:12" hidden="1">
+    <row r="44" spans="1:12">
       <c r="A44" s="19">
         <v>43</v>
       </c>
@@ -14085,7 +14079,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="45" spans="1:12" hidden="1">
+    <row r="45" spans="1:12">
       <c r="A45" s="19">
         <v>44</v>
       </c>
@@ -14115,7 +14109,7 @@
         <v>1022</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="24" hidden="1">
+    <row r="46" spans="1:12" ht="24">
       <c r="A46" s="19">
         <v>45</v>
       </c>
@@ -14149,7 +14143,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="24" hidden="1">
+    <row r="47" spans="1:12" ht="24">
       <c r="A47" s="19">
         <v>46</v>
       </c>
@@ -14183,7 +14177,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="48" spans="1:12" hidden="1">
+    <row r="48" spans="1:12">
       <c r="A48" s="19">
         <v>47</v>
       </c>
@@ -14213,7 +14207,7 @@
         <v>1254</v>
       </c>
     </row>
-    <row r="49" spans="1:16" ht="24" hidden="1">
+    <row r="49" spans="1:16" ht="24">
       <c r="A49" s="19">
         <v>48</v>
       </c>
@@ -14245,7 +14239,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:16" hidden="1">
+    <row r="50" spans="1:16">
       <c r="A50" s="19">
         <v>49</v>
       </c>
@@ -14275,7 +14269,7 @@
         <v>1254</v>
       </c>
     </row>
-    <row r="51" spans="1:16" hidden="1">
+    <row r="51" spans="1:16">
       <c r="A51" s="19">
         <v>50</v>
       </c>
@@ -14305,7 +14299,7 @@
         <v>1254</v>
       </c>
     </row>
-    <row r="52" spans="1:16" ht="24" hidden="1">
+    <row r="52" spans="1:16" ht="24">
       <c r="A52" s="19">
         <v>51</v>
       </c>
@@ -14339,7 +14333,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="53" spans="1:16" hidden="1">
+    <row r="53" spans="1:16">
       <c r="A53" s="19">
         <v>52</v>
       </c>
@@ -14367,7 +14361,7 @@
       <c r="K53" s="15"/>
       <c r="L53" s="6"/>
     </row>
-    <row r="54" spans="1:16" hidden="1">
+    <row r="54" spans="1:16">
       <c r="A54" s="19">
         <v>53</v>
       </c>
@@ -14395,7 +14389,7 @@
       <c r="K54" s="15"/>
       <c r="L54" s="6"/>
     </row>
-    <row r="55" spans="1:16" hidden="1">
+    <row r="55" spans="1:16">
       <c r="A55" s="19">
         <v>54</v>
       </c>
@@ -14423,7 +14417,7 @@
       <c r="K55" s="15"/>
       <c r="L55" s="6"/>
     </row>
-    <row r="56" spans="1:16" hidden="1">
+    <row r="56" spans="1:16">
       <c r="A56" s="19">
         <v>55</v>
       </c>
@@ -14451,7 +14445,7 @@
       <c r="K56" s="15"/>
       <c r="L56" s="6"/>
     </row>
-    <row r="57" spans="1:16" hidden="1">
+    <row r="57" spans="1:16">
       <c r="A57" s="19">
         <v>56</v>
       </c>
@@ -14481,7 +14475,7 @@
       <c r="K57" s="15"/>
       <c r="L57" s="6"/>
     </row>
-    <row r="58" spans="1:16" hidden="1">
+    <row r="58" spans="1:16">
       <c r="A58" s="19">
         <v>57</v>
       </c>
@@ -14509,7 +14503,7 @@
       <c r="K58" s="15"/>
       <c r="L58" s="6"/>
     </row>
-    <row r="59" spans="1:16" hidden="1">
+    <row r="59" spans="1:16">
       <c r="A59" s="19">
         <v>58</v>
       </c>
@@ -14537,7 +14531,7 @@
       <c r="K59" s="15"/>
       <c r="L59" s="6"/>
     </row>
-    <row r="60" spans="1:16" hidden="1">
+    <row r="60" spans="1:16">
       <c r="A60" s="19">
         <v>59</v>
       </c>
@@ -14573,7 +14567,7 @@
         <v>79.599999999999994</v>
       </c>
     </row>
-    <row r="61" spans="1:16" hidden="1">
+    <row r="61" spans="1:16">
       <c r="A61" s="19">
         <v>60</v>
       </c>
@@ -14601,7 +14595,7 @@
       <c r="K61" s="15"/>
       <c r="L61" s="6"/>
     </row>
-    <row r="62" spans="1:16" hidden="1">
+    <row r="62" spans="1:16">
       <c r="A62" s="19">
         <v>61</v>
       </c>
@@ -14629,7 +14623,7 @@
       <c r="K62" s="15"/>
       <c r="L62" s="6"/>
     </row>
-    <row r="63" spans="1:16" hidden="1">
+    <row r="63" spans="1:16">
       <c r="A63" s="19">
         <v>62</v>
       </c>
@@ -14657,7 +14651,7 @@
       <c r="K63" s="15"/>
       <c r="L63" s="6"/>
     </row>
-    <row r="64" spans="1:16" hidden="1">
+    <row r="64" spans="1:16">
       <c r="A64" s="19">
         <v>63</v>
       </c>
@@ -14685,7 +14679,7 @@
       <c r="K64" s="15"/>
       <c r="L64" s="6"/>
     </row>
-    <row r="65" spans="1:12" hidden="1">
+    <row r="65" spans="1:12">
       <c r="A65" s="19">
         <v>64</v>
       </c>
@@ -14713,7 +14707,7 @@
       <c r="K65" s="15"/>
       <c r="L65" s="6"/>
     </row>
-    <row r="66" spans="1:12" hidden="1">
+    <row r="66" spans="1:12">
       <c r="A66" s="19">
         <v>65</v>
       </c>
@@ -14741,7 +14735,7 @@
       <c r="K66" s="15"/>
       <c r="L66" s="6"/>
     </row>
-    <row r="67" spans="1:12" hidden="1">
+    <row r="67" spans="1:12">
       <c r="A67" s="19">
         <v>66</v>
       </c>
@@ -14769,7 +14763,7 @@
       <c r="K67" s="15"/>
       <c r="L67" s="6"/>
     </row>
-    <row r="68" spans="1:12" hidden="1">
+    <row r="68" spans="1:12">
       <c r="A68" s="19">
         <v>67</v>
       </c>
@@ -14797,7 +14791,7 @@
       <c r="K68" s="15"/>
       <c r="L68" s="6"/>
     </row>
-    <row r="69" spans="1:12" hidden="1">
+    <row r="69" spans="1:12">
       <c r="A69" s="19">
         <v>68</v>
       </c>
@@ -14825,7 +14819,7 @@
       <c r="K69" s="15"/>
       <c r="L69" s="6"/>
     </row>
-    <row r="70" spans="1:12" hidden="1">
+    <row r="70" spans="1:12">
       <c r="A70" s="19">
         <v>69</v>
       </c>
@@ -14853,7 +14847,7 @@
       <c r="K70" s="15"/>
       <c r="L70" s="6"/>
     </row>
-    <row r="71" spans="1:12" hidden="1">
+    <row r="71" spans="1:12">
       <c r="A71" s="19">
         <v>70</v>
       </c>
@@ -14881,7 +14875,7 @@
       <c r="K71" s="15"/>
       <c r="L71" s="6"/>
     </row>
-    <row r="72" spans="1:12" ht="24" hidden="1">
+    <row r="72" spans="1:12" ht="24">
       <c r="A72" s="19">
         <v>71</v>
       </c>
@@ -14909,7 +14903,7 @@
       <c r="K72" s="15"/>
       <c r="L72" s="6"/>
     </row>
-    <row r="73" spans="1:12" hidden="1">
+    <row r="73" spans="1:12">
       <c r="A73" s="19">
         <v>72</v>
       </c>
@@ -14937,7 +14931,7 @@
       <c r="K73" s="15"/>
       <c r="L73" s="6"/>
     </row>
-    <row r="74" spans="1:12" hidden="1">
+    <row r="74" spans="1:12">
       <c r="A74" s="19">
         <v>73</v>
       </c>
@@ -14963,7 +14957,7 @@
       <c r="K74" s="15"/>
       <c r="L74" s="6"/>
     </row>
-    <row r="75" spans="1:12" hidden="1">
+    <row r="75" spans="1:12">
       <c r="A75" s="19">
         <v>74</v>
       </c>
@@ -14991,7 +14985,7 @@
       <c r="K75" s="15"/>
       <c r="L75" s="6"/>
     </row>
-    <row r="76" spans="1:12" hidden="1">
+    <row r="76" spans="1:12">
       <c r="A76" s="19">
         <v>75</v>
       </c>
@@ -15019,7 +15013,7 @@
       <c r="K76" s="15"/>
       <c r="L76" s="6"/>
     </row>
-    <row r="77" spans="1:12" hidden="1">
+    <row r="77" spans="1:12">
       <c r="A77" s="19">
         <v>76</v>
       </c>
@@ -15047,7 +15041,7 @@
       <c r="K77" s="15"/>
       <c r="L77" s="6"/>
     </row>
-    <row r="78" spans="1:12" hidden="1">
+    <row r="78" spans="1:12">
       <c r="A78" s="19">
         <v>77</v>
       </c>
@@ -15075,7 +15069,7 @@
       <c r="K78" s="15"/>
       <c r="L78" s="6"/>
     </row>
-    <row r="79" spans="1:12" hidden="1">
+    <row r="79" spans="1:12">
       <c r="A79" s="19">
         <v>78</v>
       </c>
@@ -15103,7 +15097,7 @@
       <c r="K79" s="15"/>
       <c r="L79" s="6"/>
     </row>
-    <row r="80" spans="1:12" hidden="1">
+    <row r="80" spans="1:12">
       <c r="A80" s="19">
         <v>79</v>
       </c>
@@ -15131,7 +15125,7 @@
       <c r="K80" s="15"/>
       <c r="L80" s="6"/>
     </row>
-    <row r="81" spans="1:12" hidden="1">
+    <row r="81" spans="1:12">
       <c r="A81" s="19">
         <v>80</v>
       </c>
@@ -15159,7 +15153,7 @@
       <c r="K81" s="15"/>
       <c r="L81" s="6"/>
     </row>
-    <row r="82" spans="1:12" hidden="1">
+    <row r="82" spans="1:12">
       <c r="A82" s="19">
         <v>81</v>
       </c>
@@ -15187,7 +15181,7 @@
       <c r="K82" s="15"/>
       <c r="L82" s="6"/>
     </row>
-    <row r="83" spans="1:12" hidden="1">
+    <row r="83" spans="1:12">
       <c r="A83" s="19">
         <v>82</v>
       </c>
@@ -15215,7 +15209,7 @@
       <c r="K83" s="15"/>
       <c r="L83" s="6"/>
     </row>
-    <row r="84" spans="1:12" hidden="1">
+    <row r="84" spans="1:12">
       <c r="A84" s="19">
         <v>83</v>
       </c>
@@ -15243,7 +15237,7 @@
       <c r="K84" s="15"/>
       <c r="L84" s="6"/>
     </row>
-    <row r="85" spans="1:12" hidden="1">
+    <row r="85" spans="1:12">
       <c r="A85" s="19">
         <v>84</v>
       </c>
@@ -15271,7 +15265,7 @@
       <c r="K85" s="15"/>
       <c r="L85" s="6"/>
     </row>
-    <row r="86" spans="1:12" hidden="1">
+    <row r="86" spans="1:12">
       <c r="A86" s="19">
         <v>85</v>
       </c>
@@ -15299,7 +15293,7 @@
       <c r="K86" s="15"/>
       <c r="L86" s="6"/>
     </row>
-    <row r="87" spans="1:12" hidden="1">
+    <row r="87" spans="1:12">
       <c r="A87" s="19">
         <v>86</v>
       </c>
@@ -15327,7 +15321,7 @@
       <c r="K87" s="15"/>
       <c r="L87" s="6"/>
     </row>
-    <row r="88" spans="1:12" hidden="1">
+    <row r="88" spans="1:12">
       <c r="A88" s="19">
         <v>87</v>
       </c>
@@ -15355,7 +15349,7 @@
       <c r="K88" s="15"/>
       <c r="L88" s="6"/>
     </row>
-    <row r="89" spans="1:12" hidden="1">
+    <row r="89" spans="1:12">
       <c r="A89" s="19">
         <v>88</v>
       </c>
@@ -15383,7 +15377,7 @@
       <c r="K89" s="15"/>
       <c r="L89" s="6"/>
     </row>
-    <row r="90" spans="1:12" hidden="1">
+    <row r="90" spans="1:12">
       <c r="A90" s="19">
         <v>89</v>
       </c>
@@ -15411,7 +15405,7 @@
       <c r="K90" s="15"/>
       <c r="L90" s="6"/>
     </row>
-    <row r="91" spans="1:12" ht="36" hidden="1">
+    <row r="91" spans="1:12" ht="36">
       <c r="A91" s="19">
         <v>90</v>
       </c>
@@ -15441,7 +15435,7 @@
       <c r="K91" s="15"/>
       <c r="L91" s="6"/>
     </row>
-    <row r="92" spans="1:12" hidden="1">
+    <row r="92" spans="1:12">
       <c r="A92" s="19">
         <v>91</v>
       </c>
@@ -15469,7 +15463,7 @@
       <c r="K92" s="15"/>
       <c r="L92" s="6"/>
     </row>
-    <row r="93" spans="1:12" hidden="1">
+    <row r="93" spans="1:12">
       <c r="A93" s="19">
         <v>92</v>
       </c>
@@ -15497,7 +15491,7 @@
       <c r="K93" s="15"/>
       <c r="L93" s="6"/>
     </row>
-    <row r="94" spans="1:12" hidden="1">
+    <row r="94" spans="1:12">
       <c r="A94" s="19">
         <v>93</v>
       </c>
@@ -15525,7 +15519,7 @@
       <c r="K94" s="15"/>
       <c r="L94" s="6"/>
     </row>
-    <row r="95" spans="1:12" hidden="1">
+    <row r="95" spans="1:12">
       <c r="A95" s="19">
         <v>94</v>
       </c>
@@ -15553,7 +15547,7 @@
       <c r="K95" s="15"/>
       <c r="L95" s="6"/>
     </row>
-    <row r="96" spans="1:12" hidden="1">
+    <row r="96" spans="1:12">
       <c r="A96" s="19">
         <v>95</v>
       </c>
@@ -15721,7 +15715,7 @@
       <c r="K101" s="15"/>
       <c r="L101" s="6"/>
     </row>
-    <row r="102" spans="1:12" hidden="1">
+    <row r="102" spans="1:12">
       <c r="A102" s="19">
         <v>101</v>
       </c>
@@ -15766,7 +15760,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K254"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>